<commit_message>
updated data reading logic
</commit_message>
<xml_diff>
--- a/Data/Amazon_Data.xlsx
+++ b/Data/Amazon_Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838E7198-7BB4-41BC-8C26-48629182DE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8010EC9D-D3DE-49B3-BA90-A8FEE442A465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,18 +15,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>misalg13@gmail.com</t>
-  </si>
-  <si>
-    <t>kiaan@0407</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>searchString</t>
+  </si>
+  <si>
+    <t>searchProductString</t>
+  </si>
+  <si>
+    <t>minPriceValue</t>
+  </si>
+  <si>
+    <t>maxPriceValue</t>
+  </si>
+  <si>
+    <t>amazon</t>
+  </si>
+  <si>
+    <t>dell computers</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>dummy@email.com</t>
+  </si>
+  <si>
+    <t>dummyPass</t>
   </si>
 </sst>
 </file>
@@ -76,9 +94,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -418,39 +434,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F2" s="1">
+        <v>30000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{5952483F-0287-412F-AB08-353BB54D4AB5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>